<commit_message>
exception about 'truncate table (auditoryTypes)'
</commit_message>
<xml_diff>
--- a/data/Faculties.xlsx
+++ b/data/Faculties.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="675" yWindow="405" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>facultet</t>
   </si>
@@ -159,8 +159,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -533,27 +533,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,7 +567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="26.25">
+    <row r="2" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -581,7 +581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="26.25">
+    <row r="3" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -595,7 +595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="26.25">
+    <row r="4" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -609,7 +609,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="26.25">
+    <row r="5" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -623,7 +623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="26.25">
+    <row r="6" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -637,7 +637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="39">
+    <row r="7" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -651,7 +651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="26.25">
+    <row r="8" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -665,7 +665,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="39">
+    <row r="9" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -679,7 +679,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="39">
+    <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -693,7 +693,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="51.75">
+    <row r="11" spans="1:4" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="26.25">
+    <row r="12" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -721,7 +721,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -735,7 +735,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="39">
+    <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -749,12 +749,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>43</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>44</v>

</xml_diff>